<commit_message>
Added headphones hat and crowntiara hat
</commit_message>
<xml_diff>
--- a/Hats Spreadsheet V6.xlsx
+++ b/Hats Spreadsheet V6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\s4101141\ExperimentalGames\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\s4101141\ExperimentalGames\ExperimentalGames\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715BC92-FF60-4D52-88EE-16555D7807CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA6F00E-777B-47F5-8EA2-A1A7A84BB247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3EB3C7D8-FC78-4C7F-BA3B-069845290569}"/>
   </bookViews>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7122BC-1FA8-4F8A-8E88-D6846949F0A0}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +837,8 @@
         <v>8</v>
       </c>
       <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>78</v>
       </c>
@@ -1319,6 +1321,8 @@
         <v>63</v>
       </c>
       <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
       <c r="E62" t="s">
         <v>78</v>
       </c>

</xml_diff>